<commit_message>
prior computation + beginning posterior
</commit_message>
<xml_diff>
--- a/code/data/priors_specifications.xlsx
+++ b/code/data/priors_specifications.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Desktop\Github\GitHub\Advanced-Time-Series-Analysis-Article-Replication\code\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{93B26FF2-4D69-4A1A-9D93-DC057C1F7134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D8347B3-645A-43CC-A0C9-90AB4348FDAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{0503F735-9A9F-438D-BC8D-5ECB7561A082}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{0503F735-9A9F-438D-BC8D-5ECB7561A082}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$D$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -128,9 +131,6 @@
     <t>Mexico</t>
   </si>
   <si>
-    <t>Pery</t>
-  </si>
-  <si>
     <t>Philippines</t>
   </si>
   <si>
@@ -146,7 +146,10 @@
     <t>Thailand</t>
   </si>
   <si>
-    <t>United States of Amercia</t>
+    <t>United States of America</t>
+  </si>
+  <si>
+    <t>Peru</t>
   </si>
 </sst>
 </file>
@@ -521,7 +524,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -542,10 +545,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B2">
-        <v>5.0000000000000001E-3</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="C2">
         <v>0.01</v>
@@ -556,10 +559,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B3">
-        <v>5.0000000000000001E-3</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="C3">
         <v>0.01</v>
@@ -570,10 +573,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>5.0000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="C4">
         <v>0.01</v>
@@ -584,10 +587,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B5">
-        <v>5.0000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="C5">
         <v>0.01</v>
@@ -598,10 +601,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B6">
-        <v>1E-3</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="C6">
         <v>0.01</v>
@@ -612,10 +615,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B7">
-        <v>1E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="C7">
         <v>0.01</v>
@@ -626,10 +629,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B8">
-        <v>1E-3</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="C8">
         <v>0.01</v>
@@ -640,7 +643,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>1E-3</v>
@@ -654,10 +657,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B10">
-        <v>1E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="C10">
         <v>0.01</v>
@@ -668,7 +671,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B11">
         <v>1E-3</v>
@@ -682,7 +685,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <v>1E-3</v>
@@ -696,10 +699,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B13">
-        <v>1E-3</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="C13">
         <v>0.01</v>
@@ -710,10 +713,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B14">
-        <v>1E-3</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="C14">
         <v>0.01</v>
@@ -724,7 +727,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>1E-3</v>
@@ -738,10 +741,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B16">
-        <v>1E-3</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="C16">
         <v>0.01</v>
@@ -752,10 +755,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B17">
-        <v>1E-3</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="C17">
         <v>0.01</v>
@@ -766,7 +769,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B18">
         <v>-5.0000000000000001E-3</v>
@@ -780,10 +783,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B19">
-        <v>-5.0000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="C19">
         <v>0.01</v>
@@ -794,10 +797,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B20">
-        <v>-5.0000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="C20">
         <v>0.01</v>
@@ -808,10 +811,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B21">
-        <v>-5.0000000000000001E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="C21">
         <v>0.01</v>
@@ -822,7 +825,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="B22">
         <v>-5.0000000000000001E-3</v>
@@ -836,7 +839,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B23">
         <v>-5.0000000000000001E-3</v>
@@ -850,7 +853,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B24">
         <v>-5.0000000000000001E-3</v>
@@ -864,7 +867,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B25">
         <v>-5.0000000000000001E-3</v>
@@ -878,7 +881,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B26">
         <v>-5.0000000000000001E-3</v>
@@ -892,7 +895,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B27">
         <v>-5.0000000000000001E-3</v>
@@ -906,10 +909,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="B28">
-        <v>-5.0000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="C28">
         <v>0.01</v>
@@ -920,10 +923,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="B29">
-        <v>-5.0000000000000001E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="C29">
         <v>0.01</v>
@@ -934,10 +937,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="B30">
-        <v>-5.0000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="C30">
         <v>0.01</v>
@@ -948,7 +951,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B31">
         <v>-5.0000000000000001E-3</v>
@@ -962,10 +965,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="B32">
-        <v>-5.0000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="C32">
         <v>0.01</v>
@@ -976,10 +979,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="B33">
-        <v>-5.0000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="C33">
         <v>0.01</v>
@@ -990,7 +993,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B34">
         <v>-5.0000000000000001E-3</v>
@@ -1003,6 +1006,11 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D1" xr:uid="{7BC923C1-D0AF-4590-8AE1-B23B21203807}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D34">
+      <sortCondition ref="A1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>